<commit_message>
Added some smaller airlines
</commit_message>
<xml_diff>
--- a/data/joined/week-MAN.xlsx
+++ b/data/joined/week-MAN.xlsx
@@ -8,13 +8,45 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phil/repos/OpenDataDay2020/data/joined/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFE3E72-B770-2043-80A2-15A852D2B2CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D097EDC3-7F04-D746-9B5F-246CA1965428}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16480" xr2:uid="{C01B2760-9FBB-B442-827B-A6D965725D1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$22</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$2:$B$22</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$2:$C$22</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$D$2:$D$22</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$E$2:$E$22</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$F$2:$F$22</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$B$2:$B$22</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$C$2:$C$22</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$D$2:$D$22</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$E$2:$E$22</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$F$2:$F$22</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$2:$C$22</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$2:$D$22</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$2:$E$22</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$F$2:$F$22</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="142">
   <si>
     <t>EZY</t>
   </si>
@@ -418,6 +450,45 @@
   </si>
   <si>
     <t>Twin Town Leasing Company</t>
+  </si>
+  <si>
+    <t>Finnair</t>
+  </si>
+  <si>
+    <t>Norwegian Air Shuttle</t>
+  </si>
+  <si>
+    <t>Singapore Airlines</t>
+  </si>
+  <si>
+    <t>Pakistan International Airlines</t>
+  </si>
+  <si>
+    <t>Icelandair</t>
+  </si>
+  <si>
+    <t>Oman Air</t>
+  </si>
+  <si>
+    <t>Pegasus Airlines</t>
+  </si>
+  <si>
+    <t>TAP Portugal</t>
+  </si>
+  <si>
+    <t>United Airlines</t>
+  </si>
+  <si>
+    <t>Vueling Airlines</t>
+  </si>
+  <si>
+    <t>American Airlines</t>
+  </si>
+  <si>
+    <t>Austrian Airlines</t>
+  </si>
+  <si>
+    <t>Federal Express</t>
   </si>
 </sst>
 </file>
@@ -781,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE792A4A-D6E5-094A-B06B-6A9A7ECB3F8B}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1230,6 +1301,9 @@
       <c r="B23">
         <v>9</v>
       </c>
+      <c r="C23" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1238,6 +1312,9 @@
       <c r="B24">
         <v>9</v>
       </c>
+      <c r="C24" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1246,6 +1323,9 @@
       <c r="B25">
         <v>8</v>
       </c>
+      <c r="C25" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1254,6 +1334,9 @@
       <c r="B26">
         <v>7</v>
       </c>
+      <c r="C26" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1262,6 +1345,9 @@
       <c r="B27">
         <v>6</v>
       </c>
+      <c r="C27" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1270,6 +1356,9 @@
       <c r="B28">
         <v>6</v>
       </c>
+      <c r="C28" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1278,6 +1367,9 @@
       <c r="B29">
         <v>6</v>
       </c>
+      <c r="C29" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1286,6 +1378,9 @@
       <c r="B30">
         <v>6</v>
       </c>
+      <c r="C30" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1294,6 +1389,9 @@
       <c r="B31">
         <v>6</v>
       </c>
+      <c r="C31" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1302,24 +1400,33 @@
       <c r="B32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1327,15 +1434,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1343,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1351,7 +1461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1359,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1367,7 +1477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1375,7 +1485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1383,7 +1493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1391,7 +1501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1399,7 +1509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1407,7 +1517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1415,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1423,7 +1533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Added ESG CO2 emissions
</commit_message>
<xml_diff>
--- a/data/joined/week-MAN.xlsx
+++ b/data/joined/week-MAN.xlsx
@@ -8,45 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phil/repos/OpenDataDay2020/data/joined/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D097EDC3-7F04-D746-9B5F-246CA1965428}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1014CDE7-4973-364F-BE71-6625D6AA2754}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16480" xr2:uid="{C01B2760-9FBB-B442-827B-A6D965725D1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$22</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$2:$B$22</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$2:$C$22</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$D$2:$D$22</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$E$2:$E$22</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$F$2:$F$22</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$B$2:$B$22</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$C$2:$C$22</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$D$2:$D$22</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$E$2:$E$22</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$F$2:$F$22</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$2:$C$22</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$2:$D$22</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$2:$E$22</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$F$2:$F$22</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -63,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="152">
   <si>
     <t>EZY</t>
   </si>
@@ -489,6 +457,36 @@
   </si>
   <si>
     <t>Federal Express</t>
+  </si>
+  <si>
+    <t>RIC</t>
+  </si>
+  <si>
+    <t>CO2Ratio2018</t>
+  </si>
+  <si>
+    <t>RYA.I</t>
+  </si>
+  <si>
+    <t>LHAG.DE</t>
+  </si>
+  <si>
+    <t>FLYB.L^C19</t>
+  </si>
+  <si>
+    <t>TUIGn.DE</t>
+  </si>
+  <si>
+    <t>BAY.L^A11</t>
+  </si>
+  <si>
+    <t>AIRF.PA</t>
+  </si>
+  <si>
+    <t>ICAG.L</t>
+  </si>
+  <si>
+    <t>FIA1S.HE</t>
   </si>
 </sst>
 </file>
@@ -850,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE792A4A-D6E5-094A-B06B-6A9A7ECB3F8B}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -863,7 +861,7 @@
     <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -885,8 +883,14 @@
       <c r="G1" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -908,8 +912,14 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2">
+        <v>989.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -931,8 +941,14 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3">
+        <v>1221.9000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -954,8 +970,11 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -977,8 +996,14 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>145</v>
+      </c>
+      <c r="I5">
+        <v>847.22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -994,8 +1019,11 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1017,8 +1045,14 @@
       <c r="G7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7">
+        <v>369.42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1031,8 +1065,11 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1054,8 +1091,14 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>149</v>
+      </c>
+      <c r="I9">
+        <v>920.51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1077,8 +1120,14 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10">
+        <v>947.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1100,8 +1149,14 @@
       <c r="G11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I11">
+        <v>1074.49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1115,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1138,7 +1193,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1160,8 +1215,14 @@
       <c r="G14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14">
+        <v>920.51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1178,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1195,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1206,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1228,8 +1289,14 @@
       <c r="G18">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>145</v>
+      </c>
+      <c r="I18">
+        <v>847.22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1246,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1263,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1280,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1294,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1304,8 +1371,14 @@
       <c r="C23" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23">
+        <v>1004.68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1316,7 +1389,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1327,7 +1400,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1338,7 +1411,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1349,7 +1422,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1360,7 +1433,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1371,7 +1444,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1382,7 +1455,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1393,7 +1466,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>

</xml_diff>